<commit_message>
Update ontology_metadata.yaml & make all
</commit_message>
<xml_diff>
--- a/project/excel/ontology_metadata.xlsx
+++ b/project/excel/ontology_metadata.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:AV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,10 +458,215 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>versionInfo</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>versionIRI</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>versionNotes</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>modificationDate</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>issueTracker</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>documentation</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>imports</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>contactInfo</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>fundingInfo</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>audience</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>domainCovered</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>languageCovered</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>languageExpressedIn</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>sourceRepository</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>distributions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>applicationExample</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>references</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>citations</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>derivedFrom</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>rootTerms</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>relatedVersions</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>socialMediaAccount</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>identifierPattern</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>homepage</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>publisher</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>exampleIdentifier</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>exampleClass</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>mailingList</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>otherIdentifier</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>developmentEnvironment</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>mappingRessources</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>competencyQuestions</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>appliedMethodology</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
           <t>alternativeTitle</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>alternativePrefix</t>
         </is>
@@ -478,7 +683,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:AV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,10 +719,215 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>versionInfo</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>versionIRI</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>versionNotes</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>modificationDate</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>issueTracker</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>documentation</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>imports</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>contactInfo</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>fundingInfo</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>audience</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>domainCovered</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>languageCovered</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>languageExpressedIn</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>sourceRepository</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>distributions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>applicationExample</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>references</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>citations</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>derivedFrom</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>rootTerms</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>relatedVersions</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>socialMediaAccount</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>identifierPattern</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>homepage</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>publisher</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>exampleIdentifier</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>exampleClass</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>mailingList</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>otherIdentifier</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>developmentEnvironment</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>mappingRessources</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>competencyQuestions</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>appliedMethodology</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
           <t>alternativeTitle</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>alternativePrefix</t>
         </is>
@@ -534,14 +944,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>relatedVersions</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>socialMediaAccount</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>identifierPattern</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>homepage</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>publisher</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>exampleIdentifier</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>exampleClass</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mailingList</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>otherIdentifier</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>developmentEnvironment</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>mappingRessources</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>competencyQuestions</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>appliedMethodology</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>alternativeTitle</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>alternativePrefix</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -552,7 +1055,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -563,12 +1066,77 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>alternativeTitle</t>
+          <t>contributor</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>alternativePrefix</t>
+          <t>contactInfo</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>fundingInfo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>audience</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>domainCovered</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>languageCovered</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>languageExpressedIn</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>sourceRepository</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>distributions</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>applicationExample</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>references</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>citations</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>derivedFrom</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>rootTerms</t>
         </is>
       </c>
     </row>
@@ -583,7 +1151,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,6 +1183,56 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>license</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>versionInfo</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>versionIRI</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>versionNotes</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>modificationDate</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>issueTracker</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>documentation</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>imports</t>
         </is>
       </c>
     </row>
@@ -629,7 +1247,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:AV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,10 +1283,215 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>versionInfo</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>versionIRI</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>versionNotes</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>modificationDate</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>issueTracker</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>documentation</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>imports</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>contactInfo</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>fundingInfo</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>audience</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>domainCovered</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>languageCovered</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>languageExpressedIn</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>sourceRepository</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>distributions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>applicationExample</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>references</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>citations</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>derivedFrom</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>rootTerms</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>relatedVersions</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>socialMediaAccount</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>identifierPattern</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>homepage</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>publisher</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>exampleIdentifier</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>exampleClass</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>mailingList</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>otherIdentifier</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>developmentEnvironment</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>mappingRessources</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>competencyQuestions</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>appliedMethodology</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
           <t>alternativeTitle</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>alternativePrefix</t>
         </is>
@@ -685,7 +1508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:AV1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -721,10 +1544,215 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>versionInfo</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>versionIRI</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>versionNotes</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>modificationDate</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>issueTracker</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>documentation</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>imports</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>contributor</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>contactInfo</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>fundingInfo</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>audience</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>domainCovered</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>languageCovered</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>languageExpressedIn</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>sourceRepository</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>distributions</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>applicationExample</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>references</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>citations</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>derivedFrom</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>rootTerms</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>relatedVersions</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>socialMediaAccount</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>identifierPattern</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>homepage</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>publisher</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>exampleIdentifier</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>exampleClass</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>mailingList</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>otherIdentifier</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>developmentEnvironment</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>mappingRessources</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>competencyQuestions</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>appliedMethodology</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
           <t>alternativeTitle</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>alternativePrefix</t>
         </is>
@@ -741,14 +1769,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>relatedVersions</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>socialMediaAccount</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>identifierPattern</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>format</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>homepage</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>publisher</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>exampleIdentifier</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>exampleClass</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>mailingList</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>logo</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>otherIdentifier</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>developmentEnvironment</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>mappingRessources</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>competencyQuestions</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>appliedMethodology</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>alternativeTitle</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>alternativePrefix</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -759,7 +1880,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -770,12 +1891,77 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>alternativeTitle</t>
+          <t>contributor</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>alternativePrefix</t>
+          <t>contactInfo</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>fundingInfo</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>audience</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>domainCovered</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>languageCovered</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>languageExpressedIn</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>sourceRepository</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>distributions</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>applicationExample</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>references</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>citations</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>derivedFrom</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>rootTerms</t>
         </is>
       </c>
     </row>
@@ -790,7 +1976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -824,6 +2010,56 @@
           <t>license</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>creator</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>versionInfo</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>versionIRI</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>versionNotes</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>modificationDate</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>issueTracker</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>documentation</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>imports</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>